<commit_message>
Reorden de archivos y cambio de nombres
</commit_message>
<xml_diff>
--- a/CouriersCR/data/distinctValues.xlsx
+++ b/CouriersCR/data/distinctValues.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -2721,6 +2721,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>